<commit_message>
Archivos para pareamiento probabilístico en día 3
</commit_message>
<xml_diff>
--- a/data/pareamiento/rnve.xlsx
+++ b/data/pareamiento/rnve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://paho.sharepoint.com/sites/CIM/Meetings Presentation Library/curso_R/CIM_avanzado/data/uruguay/pareamiento/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icedu\Documents\curso-R-avanzado\data\pareamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_F7681CC78F79A8536E3CA493EA7BD272DA4C673A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E9A85F-CEBB-4C17-A20A-12547B98E440}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8F633D-3C83-45F0-8731-3DE2BA89DD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>sexo_original</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -649,26 +652,26 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -744,7 +747,7 @@
         <v>43311</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -782,7 +785,7 @@
         <v>43150</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -820,7 +823,7 @@
         <v>43290</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -858,7 +861,7 @@
         <v>43273</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -896,7 +899,7 @@
         <v>43649</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -934,7 +937,7 @@
         <v>43793</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -972,7 +975,7 @@
         <v>44030</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>43956</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>44208</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>44759</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1140,6 +1143,9 @@
       <c r="E13" t="s">
         <v>49</v>
       </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
       <c r="G13" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>44910</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1241,6 +1247,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AssessmentDone xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15" xsi:nil="true"/>
+    <h4d5a6f5320548c887a9ca0b433eca60 xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h4d5a6f5320548c887a9ca0b433eca60>
+    <SectionDone xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="63f513c6-35fa-4931-8c50-b609e7189350" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028ECBC918D5D1D48BC253772FA4A2A2A" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3bc5fc8ce9af08f171c5473651c8b843">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4989f34c-53b6-4c13-92d3-20e963bdea15" xmlns:ns3="63f513c6-35fa-4931-8c50-b609e7189350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e50e0dc527af8123b5da5903c8a1dcba" ns2:_="" ns3:_="">
     <xsd:import namespace="4989f34c-53b6-4c13-92d3-20e963bdea15"/>
@@ -1516,39 +1547,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AssessmentDone xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15" xsi:nil="true"/>
-    <h4d5a6f5320548c887a9ca0b433eca60 xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h4d5a6f5320548c887a9ca0b433eca60>
-    <SectionDone xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4989f34c-53b6-4c13-92d3-20e963bdea15">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="63f513c6-35fa-4931-8c50-b609e7189350" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8F5452C-A12B-473C-83E0-C3918AA8D6B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66700F8C-66B1-48A0-B992-84C2279CBD0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4989f34c-53b6-4c13-92d3-20e963bdea15"/>
+    <ds:schemaRef ds:uri="63f513c6-35fa-4931-8c50-b609e7189350"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F4F3BC-EB81-4B20-AA99-4C43FB49AD99}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F4F3BC-EB81-4B20-AA99-4C43FB49AD99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66700F8C-66B1-48A0-B992-84C2279CBD0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8F5452C-A12B-473C-83E0-C3918AA8D6B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4989f34c-53b6-4c13-92d3-20e963bdea15"/>
+    <ds:schemaRef ds:uri="63f513c6-35fa-4931-8c50-b609e7189350"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>